<commit_message>
Did some stuff I think..
</commit_message>
<xml_diff>
--- a/GlobalReserves/BalSheets/CNCBBS.xlsx
+++ b/GlobalReserves/BalSheets/CNCBBS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="8">
   <si>
     <t>symbol</t>
   </si>
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G313"/>
+  <dimension ref="A1:G317"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7587,6 +7587,9 @@
       <c r="A313" s="2">
         <v>45230</v>
       </c>
+      <c r="B313" t="s">
+        <v>7</v>
+      </c>
       <c r="C313">
         <v>43325980000000</v>
       </c>
@@ -7600,6 +7603,95 @@
         <v>43325980000000</v>
       </c>
       <c r="G313">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7">
+      <c r="A314" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B314" t="s">
+        <v>7</v>
+      </c>
+      <c r="C314">
+        <v>43325980000000</v>
+      </c>
+      <c r="D314">
+        <v>43325980000000</v>
+      </c>
+      <c r="E314">
+        <v>43325980000000</v>
+      </c>
+      <c r="F314">
+        <v>43325980000000</v>
+      </c>
+      <c r="G314">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7">
+      <c r="A315" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B315" t="s">
+        <v>7</v>
+      </c>
+      <c r="C315">
+        <v>43325980000000</v>
+      </c>
+      <c r="D315">
+        <v>43325980000000</v>
+      </c>
+      <c r="E315">
+        <v>43325980000000</v>
+      </c>
+      <c r="F315">
+        <v>43325980000000</v>
+      </c>
+      <c r="G315">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7">
+      <c r="A316" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B316" t="s">
+        <v>7</v>
+      </c>
+      <c r="C316">
+        <v>43325980000000</v>
+      </c>
+      <c r="D316">
+        <v>43325980000000</v>
+      </c>
+      <c r="E316">
+        <v>43325980000000</v>
+      </c>
+      <c r="F316">
+        <v>43325980000000</v>
+      </c>
+      <c r="G316">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7">
+      <c r="A317" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C317">
+        <v>43325980000000</v>
+      </c>
+      <c r="D317">
+        <v>43325980000000</v>
+      </c>
+      <c r="E317">
+        <v>43325980000000</v>
+      </c>
+      <c r="F317">
+        <v>43325980000000</v>
+      </c>
+      <c r="G317">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Significant upgrades of NLQ script and others.
</commit_message>
<xml_diff>
--- a/GlobalReserves/BalSheets/CNCBBS.xlsx
+++ b/GlobalReserves/BalSheets/CNCBBS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="8">
   <si>
     <t>symbol</t>
   </si>
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G317"/>
+  <dimension ref="A1:G326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7679,6 +7679,9 @@
       <c r="A317" s="2">
         <v>45230</v>
       </c>
+      <c r="B317" t="s">
+        <v>7</v>
+      </c>
       <c r="C317">
         <v>43325980000000</v>
       </c>
@@ -7692,6 +7695,210 @@
         <v>43325980000000</v>
       </c>
       <c r="G317">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7">
+      <c r="A318" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B318" t="s">
+        <v>7</v>
+      </c>
+      <c r="C318">
+        <v>43325980000000</v>
+      </c>
+      <c r="D318">
+        <v>43325980000000</v>
+      </c>
+      <c r="E318">
+        <v>43325980000000</v>
+      </c>
+      <c r="F318">
+        <v>43325980000000</v>
+      </c>
+      <c r="G318">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7">
+      <c r="A319" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B319" t="s">
+        <v>7</v>
+      </c>
+      <c r="C319">
+        <v>44065463000000</v>
+      </c>
+      <c r="D319">
+        <v>44065463000000</v>
+      </c>
+      <c r="E319">
+        <v>44065463000000</v>
+      </c>
+      <c r="F319">
+        <v>44065463000000</v>
+      </c>
+      <c r="G319">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7">
+      <c r="A320" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B320" t="s">
+        <v>7</v>
+      </c>
+      <c r="C320">
+        <v>44065463000000</v>
+      </c>
+      <c r="D320">
+        <v>44065463000000</v>
+      </c>
+      <c r="E320">
+        <v>44065463000000</v>
+      </c>
+      <c r="F320">
+        <v>44065463000000</v>
+      </c>
+      <c r="G320">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7">
+      <c r="A321" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B321" t="s">
+        <v>7</v>
+      </c>
+      <c r="C321">
+        <v>44065463000000</v>
+      </c>
+      <c r="D321">
+        <v>44065463000000</v>
+      </c>
+      <c r="E321">
+        <v>44065463000000</v>
+      </c>
+      <c r="F321">
+        <v>44065463000000</v>
+      </c>
+      <c r="G321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7">
+      <c r="A322" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B322" t="s">
+        <v>7</v>
+      </c>
+      <c r="C322">
+        <v>44065463000000</v>
+      </c>
+      <c r="D322">
+        <v>44065463000000</v>
+      </c>
+      <c r="E322">
+        <v>44065463000000</v>
+      </c>
+      <c r="F322">
+        <v>44065463000000</v>
+      </c>
+      <c r="G322">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7">
+      <c r="A323" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B323" t="s">
+        <v>7</v>
+      </c>
+      <c r="C323">
+        <v>44065463000000</v>
+      </c>
+      <c r="D323">
+        <v>44065463000000</v>
+      </c>
+      <c r="E323">
+        <v>44065463000000</v>
+      </c>
+      <c r="F323">
+        <v>44065463000000</v>
+      </c>
+      <c r="G323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7">
+      <c r="A324" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B324" t="s">
+        <v>7</v>
+      </c>
+      <c r="C324">
+        <v>44065463000000</v>
+      </c>
+      <c r="D324">
+        <v>44065463000000</v>
+      </c>
+      <c r="E324">
+        <v>44065463000000</v>
+      </c>
+      <c r="F324">
+        <v>44065463000000</v>
+      </c>
+      <c r="G324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7">
+      <c r="A325" s="2">
+        <v>45257</v>
+      </c>
+      <c r="B325" t="s">
+        <v>7</v>
+      </c>
+      <c r="C325">
+        <v>44065463000000</v>
+      </c>
+      <c r="D325">
+        <v>44065463000000</v>
+      </c>
+      <c r="E325">
+        <v>44065463000000</v>
+      </c>
+      <c r="F325">
+        <v>44065463000000</v>
+      </c>
+      <c r="G325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7">
+      <c r="A326" s="2">
+        <v>45257</v>
+      </c>
+      <c r="C326">
+        <v>44065463000000</v>
+      </c>
+      <c r="D326">
+        <v>44065463000000</v>
+      </c>
+      <c r="E326">
+        <v>44065463000000</v>
+      </c>
+      <c r="F326">
+        <v>44065463000000</v>
+      </c>
+      <c r="G326">
         <v>0</v>
       </c>
     </row>

</xml_diff>